<commit_message>
Codes merged to run on device and emulator
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\eclipse-workspace\Appium Workspace\Training Workspace\appiumemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C620C62-4AD3-4CE1-AEB0-2CEAF99B097F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8EE7CC-5CB1-40BE-848D-0335A706FFCE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16590" windowHeight="4170" xr2:uid="{A318CCDC-E660-446A-8433-F6059CCB12E5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16590" windowHeight="4170" activeTab="3" xr2:uid="{A318CCDC-E660-446A-8433-F6059CCB12E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Swetha" sheetId="3" r:id="rId2"/>
-    <sheet name="Mohan" sheetId="1" r:id="rId3"/>
-    <sheet name="EMI" sheetId="2" r:id="rId4"/>
+    <sheet name="Moha1" sheetId="1" r:id="rId3"/>
+    <sheet name="Mohan" sheetId="5" r:id="rId4"/>
+    <sheet name="EMI" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Search Txet</t>
   </si>
@@ -58,15 +59,6 @@
   </si>
   <si>
     <t>takeout</t>
-  </si>
-  <si>
-    <t>breadbox</t>
-  </si>
-  <si>
-    <t>readopt</t>
-  </si>
-  <si>
-    <t>discoverably</t>
   </si>
   <si>
     <t>Flat Loan</t>
@@ -472,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4845B3-C910-499E-975D-81857895CEAC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,15 +475,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>2000</v>
@@ -499,7 +491,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2000</v>
@@ -507,7 +499,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -533,27 +525,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +558,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,28 +607,13 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -644,6 +621,61 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41B80A0-6E0F-4CDF-BAA8-9D2C68041C99}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E737E10A-F478-4B51-BE10-57A84662531D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -658,13 +690,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,7 +729,7 @@
         <v>7.2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,7 +751,7 @@
         <v>6.2</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new code by shambhu
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\eclipse-workspace\Appium Workspace\Training Workspace\appiumemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TestNG_Project\New Project\VULCAN_APPIUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717E423-2D41-4D18-B7B3-F51FB04F390A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA75B6-462F-46DF-8DD6-E6DE806E65EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16590" windowHeight="4170" activeTab="1" xr2:uid="{A318CCDC-E660-446A-8433-F6059CCB12E5}"/>
+    <workbookView xWindow="540" yWindow="3810" windowWidth="19920" windowHeight="7110" activeTab="2" xr2:uid="{A318CCDC-E660-446A-8433-F6059CCB12E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Mohan" sheetId="1" r:id="rId1"/>
     <sheet name="EMI" sheetId="2" r:id="rId2"/>
+    <sheet name="Wheel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Search Txet</t>
   </si>
@@ -89,6 +90,27 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Maker</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Trim</t>
+  </si>
+  <si>
+    <t>Grip</t>
+  </si>
+  <si>
+    <t>AZ05</t>
+  </si>
+  <si>
+    <t>Apollo</t>
   </si>
 </sst>
 </file>
@@ -525,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E737E10A-F478-4B51-BE10-57A84662531D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -603,4 +625,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049B40B8-81CF-4D77-AE37-132D192F1540}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>